<commit_message>
fixed crash issue and full model NULL results issue
</commit_message>
<xml_diff>
--- a/Additional files/Datasets/general/dose_to_serum_data.xlsx
+++ b/Additional files/Datasets/general/dose_to_serum_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oehhacloud-my.sharepoint.com/personal/scott_coffin_oehha_ca_gov/Documents/R_new/PFHpA/output/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oehhacloud-my.sharepoint.com/personal/scott_coffin_oehha_ca_gov/Documents/R_new/PFOS_PBPK_fork/Additional files/Datasets/general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_B545C19001982AEE2F3677A119FDBA11F879DAE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{345654B5-5AD0-43DA-A2B7-7F56500BDA15}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_B545C19001982AEE2F3677A119FDBA11F879DAE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{816AF0A1-61F1-4E92-AAC5-B142A493723B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matched TK Data" sheetId="1" r:id="rId1"/>
@@ -701,8 +701,47 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12ECA2AC-BC5C-4A1E-B815-F2AB47203571}" name="Table1" displayName="Table1" ref="A1:AH42" totalsRowShown="0">
+  <autoFilter ref="A1:AH42" xr:uid="{12ECA2AC-BC5C-4A1E-B815-F2AB47203571}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{F751DA53-8C53-4493-91EF-1C7139C5CC1B}" name="Study"/>
+    <tableColumn id="2" xr3:uid="{8ACE5470-BB4F-4D78-AFB9-E902914ADC72}" name="chem"/>
+    <tableColumn id="3" xr3:uid="{AC4D5AD4-ACF6-4291-A9F1-1450DA934562}" name="sex"/>
+    <tableColumn id="4" xr3:uid="{74BCB744-30AF-46BE-9343-900AFB74A865}" name="species_name"/>
+    <tableColumn id="5" xr3:uid="{47CCF2E9-9571-400F-B2D1-7E0887DBC99B}" name="route"/>
+    <tableColumn id="6" xr3:uid="{5D87898B-F20B-41AD-9CDC-4AE6673A0EF4}" name="strain"/>
+    <tableColumn id="7" xr3:uid="{C8850A10-8EBE-43C6-B8BC-C3DBCE1D11D3}" name="CLTot_L_kg_day"/>
+    <tableColumn id="8" xr3:uid="{22BE880A-DE18-4F2A-BEA8-B4ABC2B3941A}" name="pubmed_CL"/>
+    <tableColumn id="9" xr3:uid="{B4DEB03C-D676-40EC-8228-BA12878CC958}" name="author_year_CL"/>
+    <tableColumn id="10" xr3:uid="{4DAE3B6E-43E5-4226-BC9B-A7A3C8AB20B9}" name="tissue_CL"/>
+    <tableColumn id="11" xr3:uid="{9857CDC6-1D52-42F0-8488-EA3D5E4683C1}" name="route_CL"/>
+    <tableColumn id="12" xr3:uid="{5B33E145-D2CA-4C5C-9CCE-26446A3C3BEE}" name="strain_CL"/>
+    <tableColumn id="13" xr3:uid="{5FC686CB-0D98-4977-82D9-228A8D75F3CA}" name="mismatches_CL"/>
+    <tableColumn id="14" xr3:uid="{F052FECA-0E6B-440B-9CEA-C49823B471D1}" name="VDss_L_kg"/>
+    <tableColumn id="15" xr3:uid="{DFDE1DC7-EBD5-46FA-919D-A622109E91C8}" name="pubmed_VDss"/>
+    <tableColumn id="16" xr3:uid="{C1C94DFA-A253-46D2-88B9-D2CCCDE7AA65}" name="author_year_VDss"/>
+    <tableColumn id="17" xr3:uid="{BC973464-78E2-4200-8B67-A11F36197080}" name="tissue_VDss"/>
+    <tableColumn id="18" xr3:uid="{8AEBF824-E2A1-46ED-9F59-7E25975960AB}" name="route_VDss"/>
+    <tableColumn id="19" xr3:uid="{0A442FDA-DE3A-4F5A-A2E2-BE440AFAA1B8}" name="strain_VDss"/>
+    <tableColumn id="20" xr3:uid="{92A6ED74-78E1-40A1-8151-F0B54A0557FD}" name="mismatches_VDss"/>
+    <tableColumn id="21" xr3:uid="{C275151A-5ABC-4CC3-83D1-0349A88627AC}" name="HLe_invivo"/>
+    <tableColumn id="22" xr3:uid="{DCFC61D5-951D-4CF9-A6B3-23F634040788}" name="pubmed_HLe"/>
+    <tableColumn id="23" xr3:uid="{59F66F79-A5A1-4F9D-BB5A-1F5E7D3CBA48}" name="author_year_HLe"/>
+    <tableColumn id="24" xr3:uid="{66B9091F-F6B8-46B9-9B86-A89866E91405}" name="tissue_HLe"/>
+    <tableColumn id="25" xr3:uid="{3BCE1555-566B-48A9-8AC4-212BCB7F6C1F}" name="route_HLe"/>
+    <tableColumn id="26" xr3:uid="{020A275A-502F-4E3D-917E-C2F248787DC1}" name="strain_HLe"/>
+    <tableColumn id="27" xr3:uid="{0B6FCBBC-DF4B-40E2-A898-CEE163F4669B}" name="mismatches_HLe"/>
+    <tableColumn id="28" xr3:uid="{74C73DB6-6BF2-4E4F-82B7-25D6C2E6DD19}" name="kabs"/>
+    <tableColumn id="29" xr3:uid="{52A127FD-11B7-4446-A237-440B4AD105AA}" name="pubmed_kabs"/>
+    <tableColumn id="30" xr3:uid="{EFA7950C-DC42-44F4-9902-AE1AAB2647A7}" name="author_year_kabs"/>
+    <tableColumn id="31" xr3:uid="{3FCE377F-685B-4826-A4D5-8792A6D0FB03}" name="tissue_kabs"/>
+    <tableColumn id="32" xr3:uid="{027AB19B-3919-4747-BDE7-EF0FF037BD28}" name="route_kabs"/>
+    <tableColumn id="33" xr3:uid="{07CCBE07-12E8-4912-8E32-83CD8EEC308D}" name="strain_kabs"/>
+    <tableColumn id="34" xr3:uid="{69C35F48-561C-40DC-B207-FFD408DF1787}" name="mismatches_kabs"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -987,15 +1026,38 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection sqref="A1:AH42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="18.21875" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" customWidth="1"/>
+    <col min="20" max="20" width="17.88671875" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" customWidth="1"/>
+    <col min="22" max="22" width="14.109375" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="11.77734375" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" customWidth="1"/>
+    <col min="27" max="27" width="17" customWidth="1"/>
+    <col min="29" max="29" width="14.88671875" customWidth="1"/>
+    <col min="30" max="30" width="18.109375" customWidth="1"/>
+    <col min="31" max="31" width="12.5546875" customWidth="1"/>
+    <col min="32" max="32" width="12.33203125" customWidth="1"/>
+    <col min="33" max="33" width="12.44140625" customWidth="1"/>
+    <col min="34" max="34" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1158,7 +1220,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1217,7 +1279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1282,7 +1344,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1368,7 +1430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1451,7 +1513,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1537,7 +1599,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1623,7 +1685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1709,7 +1771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -1795,7 +1857,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1881,7 +1943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -1985,7 +2047,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -2089,7 +2151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -2193,7 +2255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2279,7 +2341,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -2365,7 +2427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -2451,7 +2513,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2537,7 +2599,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -2623,7 +2685,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2727,7 +2789,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>115</v>
       </c>
@@ -2813,7 +2875,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -2899,7 +2961,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -2985,7 +3047,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -3071,7 +3133,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -3157,7 +3219,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -3243,7 +3305,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -3329,7 +3391,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -3415,7 +3477,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -3501,7 +3563,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -3587,7 +3649,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3673,7 +3735,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -3759,7 +3821,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -3845,7 +3907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -3949,7 +4011,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -4035,7 +4097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -4121,7 +4183,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -4207,7 +4269,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>104</v>
       </c>
@@ -4293,7 +4355,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>140</v>
       </c>
@@ -4397,7 +4459,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>141</v>
       </c>
@@ -4429,7 +4491,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -4461,7 +4523,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -4496,6 +4558,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4507,9 +4572,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4553,7 +4618,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -4597,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -4641,7 +4706,7 @@
         <v>0.37961613216715301</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -4685,7 +4750,7 @@
         <v>0.75923226433430502</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -4729,7 +4794,7 @@
         <v>1.51846452866861</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -4773,7 +4838,7 @@
         <v>3.0369290573372201</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -4817,7 +4882,7 @@
         <v>6.0738581146744401</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -4861,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -4905,7 +4970,7 @@
         <v>1.77154195011338</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -4949,7 +5014,7 @@
         <v>3.54308390022676</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -4993,7 +5058,7 @@
         <v>7.0861678004535102</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -5037,7 +5102,7 @@
         <v>14.172335600906999</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -5081,7 +5146,7 @@
         <v>28.344671201814101</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -5125,7 +5190,7 @@
         <v>32.597970115590599</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -5169,7 +5234,7 @@
         <v>4.8945901074460396</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -5213,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -5257,7 +5322,7 @@
         <v>1.8599292589191601</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -5301,7 +5366,7 @@
         <v>9.2996462945957905</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -5345,7 +5410,7 @@
         <v>18.599292589191599</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -5389,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -5433,7 +5498,7 @@
         <v>1.0915015068957901</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -5477,7 +5542,7 @@
         <v>5.4575075344789701</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>137</v>
       </c>
@@ -5521,7 +5586,7 @@
         <v>10.915015068957899</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -5565,7 +5630,7 @@
         <v>0.25941327569464001</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -5609,7 +5674,7 @@
         <v>1.24322588729129</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -5653,7 +5718,7 @@
         <v>6.3727563198947497</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -5697,7 +5762,7 @@
         <v>7.4868908778591398E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -5741,7 +5806,7 @@
         <v>0.35880571376909898</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -5785,7 +5850,7 @@
         <v>1.83923243829672</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -5829,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -5873,7 +5938,7 @@
         <v>38.548752834467102</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -5917,7 +5982,7 @@
         <v>3.6848072562358301</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -5961,7 +6026,7 @@
         <v>40.249433106575999</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -6005,7 +6070,7 @@
         <v>9.7181729834791106E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -6049,7 +6114,7 @@
         <v>0.97789115646258495</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -6093,7 +6158,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -6137,7 +6202,7 @@
         <v>2.6041666666666701</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -6181,7 +6246,7 @@
         <v>5.2083333333333304</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -6225,7 +6290,7 @@
         <v>10.4166666666667</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -6269,7 +6334,7 @@
         <v>20.8333333333333</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -6313,7 +6378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -6357,7 +6422,7 @@
         <v>285.24433345016899</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -6401,7 +6466,7 @@
         <v>570.48866690033901</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -6445,7 +6510,7 @@
         <v>1140.9773338006801</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -6489,7 +6554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>121</v>
       </c>
@@ -6533,7 +6598,7 @@
         <v>0.263366370010787</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>121</v>
       </c>
@@ -6577,7 +6642,7 @@
         <v>0.526732740021575</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -6621,7 +6686,7 @@
         <v>1.05346548004315</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -6659,7 +6724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -6697,7 +6762,7 @@
         <v>23.12</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -6735,7 +6800,7 @@
         <v>57.81</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -6779,7 +6844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>128</v>
       </c>
@@ -6823,7 +6888,7 @@
         <v>0.56752248331882804</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -6867,7 +6932,7 @@
         <v>1.13323179576443</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>128</v>
       </c>
@@ -6911,7 +6976,7 @@
         <v>2.2664635915288698</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -6955,7 +7020,7 @@
         <v>4.5329271830577298</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -6999,7 +7064,7 @@
         <v>9.0658543661154596</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -7043,7 +7108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -7087,7 +7152,7 @@
         <v>1.33350374914792</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -7131,7 +7196,7 @@
         <v>2.6627471029311498</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -7175,7 +7240,7 @@
         <v>5.3254942058622996</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>128</v>
       </c>
@@ -7219,7 +7284,7 @@
         <v>10.650988411724599</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -7263,7 +7328,7 @@
         <v>21.301976823449198</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -7307,7 +7372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -7351,7 +7416,7 @@
         <v>0.104299957346982</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -7395,7 +7460,7 @@
         <v>0.20826668799317599</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -7439,7 +7504,7 @@
         <v>0.41653337598635098</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -7483,7 +7548,7 @@
         <v>0.83306675197270197</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -7527,7 +7592,7 @@
         <v>1.6661335039453999</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -7571,7 +7636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -7615,7 +7680,7 @@
         <v>0.41096825696939099</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>34</v>
       </c>
@@ -7659,7 +7724,7 @@
         <v>0.82062351631268304</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -7703,7 +7768,7 @@
         <v>1.6412470326253701</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -7747,7 +7812,7 @@
         <v>3.28249406525073</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -7791,7 +7856,7 @@
         <v>6.5649881305014599</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>34</v>
       </c>
@@ -7835,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -7879,7 +7944,7 @@
         <v>1.60066981875493</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>34</v>
       </c>
@@ -7923,7 +7988,7 @@
         <v>3.2013396375098502</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -7967,7 +8032,7 @@
         <v>6.4129399789860804</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>34</v>
       </c>
@@ -8011,7 +8076,7 @@
         <v>12.8258799579722</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -8055,7 +8120,7 @@
         <v>25.6517599159443</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>34</v>
       </c>
@@ -8099,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -8143,7 +8208,7 @@
         <v>1.5700483091787401</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>34</v>
       </c>
@@ -8187,7 +8252,7 @@
         <v>3.1400966183574899</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>34</v>
       </c>
@@ -8231,7 +8296,7 @@
         <v>6.2902576489533004</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -8275,7 +8340,7 @@
         <v>12.580515297906601</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>34</v>
       </c>
@@ -8319,7 +8384,7 @@
         <v>25.161030595813202</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>34</v>
       </c>
@@ -8363,7 +8428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>34</v>
       </c>
@@ -8407,7 +8472,7 @@
         <v>0.57035555087571499</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>34</v>
       </c>
@@ -8451,7 +8516,7 @@
         <v>1.14253916441449</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>34</v>
       </c>
@@ -8495,7 +8560,7 @@
         <v>2.2850783288289902</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>34</v>
       </c>
@@ -8539,7 +8604,7 @@
         <v>4.5701566576579697</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>34</v>
       </c>
@@ -8583,7 +8648,7 @@
         <v>9.1403133153159501</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -8627,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>34</v>
       </c>
@@ -8671,7 +8736,7 @@
         <v>2.89043538743858</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>34</v>
       </c>
@@ -8715,7 +8780,7 @@
         <v>5.7808707748771697</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -8759,7 +8824,7 @@
         <v>11.5617415497543</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>34</v>
       </c>
@@ -8803,7 +8868,7 @@
         <v>23.1234830995087</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -8847,7 +8912,7 @@
         <v>46.246966199017301</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>34</v>
       </c>
@@ -8891,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>34</v>
       </c>
@@ -8935,7 +9000,7 @@
         <v>0.61441318814277102</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>34</v>
       </c>
@@ -8979,7 +9044,7 @@
         <v>1.22882637628554</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>34</v>
       </c>
@@ -9023,7 +9088,7 @@
         <v>2.4615912986489201</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>34</v>
       </c>
@@ -9067,7 +9132,7 @@
         <v>4.9231825972978402</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>34</v>
       </c>
@@ -9111,7 +9176,7 @@
         <v>9.8463651945956805</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>34</v>
       </c>
@@ -9155,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>34</v>
       </c>
@@ -9199,7 +9264,7 @@
         <v>3.7262000152625099</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>34</v>
       </c>
@@ -9243,7 +9308,7 @@
         <v>7.4524000305250304</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>34</v>
       </c>
@@ -9287,7 +9352,7 @@
         <v>14.9048000610501</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>34</v>
       </c>
@@ -9331,7 +9396,7 @@
         <v>29.8096001221001</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -9375,7 +9440,7 @@
         <v>59.619200244200201</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -9419,7 +9484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -9463,7 +9528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>34</v>
       </c>
@@ -9507,7 +9572,7 @@
         <v>20.032051282051299</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>34</v>
       </c>
@@ -9551,7 +9616,7 @@
         <v>40.064102564102598</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>34</v>
       </c>
@@ -9595,7 +9660,7 @@
         <v>80.128205128205096</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>34</v>
       </c>
@@ -9639,7 +9704,7 @@
         <v>160.25641025640999</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>127</v>
       </c>
@@ -9683,7 +9748,7 @@
         <v>0.106509884117246</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>127</v>
       </c>
@@ -9727,7 +9792,7 @@
         <v>0.53254942058623</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -9771,7 +9836,7 @@
         <v>2.13019768234492</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>139</v>
       </c>
@@ -9815,7 +9880,7 @@
         <v>4.5329271830577299E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>139</v>
       </c>
@@ -9859,7 +9924,7 @@
         <v>0.226646359152887</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -9903,7 +9968,7 @@
         <v>0.906585436611546</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>132</v>
       </c>
@@ -9947,7 +10012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -9991,7 +10056,7 @@
         <v>182.55637340810799</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -10035,7 +10100,7 @@
         <v>456.39093352027101</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>132</v>
       </c>
@@ -10079,7 +10144,7 @@
         <v>912.78186704054201</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>132</v>
       </c>
@@ -10123,7 +10188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>132</v>
       </c>
@@ -10167,7 +10232,7 @@
         <v>118.70845204178499</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>132</v>
       </c>
@@ -10211,7 +10276,7 @@
         <v>296.771130104463</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>132</v>
       </c>
@@ -10255,7 +10320,7 @@
         <v>593.54226020892702</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>126</v>
       </c>
@@ -10299,7 +10364,7 @@
         <v>2.6627471029311501E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>126</v>
       </c>
@@ -10343,7 +10408,7 @@
         <v>0.15976482617586901</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>126</v>
       </c>
@@ -10387,7 +10452,7 @@
         <v>1.06509884117246</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>138</v>
       </c>
@@ -10431,7 +10496,7 @@
         <v>2.2664635915288701E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>138</v>
       </c>
@@ -10475,7 +10540,7 @@
         <v>0.135987815491732</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -10519,7 +10584,7 @@
         <v>0.906585436611546</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>98</v>
       </c>
@@ -10548,7 +10613,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>115</v>
       </c>
@@ -10592,7 +10657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>115</v>
       </c>
@@ -10636,7 +10701,7 @@
         <v>0.97097936863037504</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>115</v>
       </c>
@@ -10680,7 +10745,7 @@
         <v>3.8839174745215002</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>104</v>
       </c>
@@ -10724,7 +10789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>104</v>
       </c>
@@ -10768,7 +10833,7 @@
         <v>3.3934931804361002</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>104</v>
       </c>
@@ -10812,7 +10877,7 @@
         <v>13.573972721744401</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>104</v>
       </c>
@@ -10856,7 +10921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>104</v>
       </c>
@@ -10900,7 +10965,7 @@
         <v>6.4945051291003697</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>104</v>
       </c>
@@ -10944,7 +11009,7 @@
         <v>25.9780205164015</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>124</v>
       </c>
@@ -10988,7 +11053,7 @@
         <v>0.106509884117246</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>124</v>
       </c>
@@ -11032,7 +11097,7 @@
         <v>0.53254942058623</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>124</v>
       </c>
@@ -11076,7 +11141,7 @@
         <v>2.13019768234492</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>129</v>
       </c>
@@ -11120,7 +11185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>129</v>
       </c>
@@ -11164,7 +11229,7 @@
         <v>4.5639093352027098</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -11208,7 +11273,7 @@
         <v>91.278186704054207</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>129</v>
       </c>
@@ -11252,7 +11317,7 @@
         <v>456.39093352027101</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>129</v>
       </c>
@@ -11296,7 +11361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>129</v>
       </c>
@@ -11340,7 +11405,7 @@
         <v>2.9677113010446301</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>129</v>
       </c>
@@ -11384,7 +11449,7 @@
         <v>59.354226020892703</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>129</v>
       </c>
@@ -11428,7 +11493,7 @@
         <v>296.771130104463</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>141</v>
       </c>
@@ -11457,7 +11522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>141</v>
       </c>
@@ -11486,7 +11551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>141</v>
       </c>
@@ -11515,7 +11580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>141</v>
       </c>
@@ -11544,7 +11609,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>141</v>
       </c>
@@ -11573,7 +11638,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>141</v>
       </c>
@@ -11602,7 +11667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>141</v>
       </c>
@@ -11631,7 +11696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>141</v>
       </c>
@@ -11660,7 +11725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>141</v>
       </c>
@@ -11689,7 +11754,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>141</v>
       </c>
@@ -11735,9 +11800,9 @@
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11814,7 +11879,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -11885,7 +11950,7 @@
         <v>99.2767647058824</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -11956,7 +12021,7 @@
         <v>99.314534883720896</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -12027,7 +12092,7 @@
         <v>99.413495145631103</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -12098,7 +12163,7 @@
         <v>30.912778904665299</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -12169,7 +12234,7 @@
         <v>-114.537329127234</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -12240,7 +12305,7 @@
         <v>-408.88077858880803</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -12314,7 +12379,7 @@
         <v>22.093023255814</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -12388,7 +12453,7 @@
         <v>-207.24770642201801</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -12462,7 +12527,7 @@
         <v>-472.47863247863199</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -12530,7 +12595,7 @@
         <v>96.740563211503897</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -12598,7 +12663,7 @@
         <v>95.273675065160703</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -12666,7 +12731,7 @@
         <v>93.253488372093003</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -12734,7 +12799,7 @@
         <v>89.233147804576404</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -12802,7 +12867,7 @@
         <v>82.472306143001006</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -12870,7 +12935,7 @@
         <v>86.2057790980286</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -12938,7 +13003,7 @@
         <v>79.706407458837504</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -13006,7 +13071,7 @@
         <v>67.941084299592603</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -13074,7 +13139,7 @@
         <v>51.193032689095702</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -13142,7 +13207,7 @@
         <v>14.3335776358497</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -13210,7 +13275,7 @@
         <v>-190.21164021164</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -13278,7 +13343,7 @@
         <v>-335.58648111332002</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -13346,7 +13411,7 @@
         <v>-237.93369313801099</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -13414,7 +13479,7 @@
         <v>-162.50374363581901</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -13482,7 +13547,7 @@
         <v>-60.825688073394502</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -13550,7 +13615,7 @@
         <v>65.410852713178301</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -13618,7 +13683,7 @@
         <v>69.489726027397296</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -13686,7 +13751,7 @@
         <v>62.484210526315799</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -13754,7 +13819,7 @@
         <v>78.639088729016805</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -13822,7 +13887,7 @@
         <v>89.381704410011906</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -13893,7 +13958,7 @@
         <v>-4433.6048879837099</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -13964,7 +14029,7 @@
         <v>-3761.23156981787</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -14035,7 +14100,7 @@
         <v>-2908.4459459459499</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -14106,7 +14171,7 @@
         <v>-1809.7147758953499</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -14177,7 +14242,7 @@
         <v>-1419.6245733788401</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -14248,7 +14313,7 @@
         <v>99.596370092720406</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -14319,7 +14384,7 @@
         <v>99.443113772455106</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -14390,7 +14455,7 @@
         <v>99.142512836634197</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -14461,7 +14526,7 @@
         <v>98.521228545618797</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -14532,7 +14597,7 @@
         <v>97.797442799461606</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -14603,7 +14668,7 @@
         <v>75.133858267716505</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -14674,7 +14739,7 @@
         <v>66.126609442060101</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -14745,7 +14810,7 @@
         <v>54.640804597701099</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -14816,7 +14881,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -14887,7 +14952,7 @@
         <v>0.22580645161290699</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>121</v>
       </c>
@@ -14958,7 +15023,7 @@
         <v>-37.488888888888901</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -15029,7 +15094,7 @@
         <v>59.232804232804199</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>137</v>
       </c>
@@ -15100,7 +15165,7 @@
         <v>-73.581081081081095</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -15171,7 +15236,7 @@
         <v>-518.87550200803196</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -15242,7 +15307,7 @@
         <v>97.971344289928396</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -15313,7 +15378,7 @@
         <v>98.129557796741693</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -15384,7 +15449,7 @@
         <v>97.953532781667704</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -15455,7 +15520,7 @@
         <v>97.779504893494504</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -15526,7 +15591,7 @@
         <v>97.575424261470801</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -15594,7 +15659,7 @@
         <v>98.105142482803799</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -15662,7 +15727,7 @@
         <v>98.269374346722401</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -15730,7 +15795,7 @@
         <v>98.284233900814201</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -15798,7 +15863,7 @@
         <v>98.048421052631596</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -15866,7 +15931,7 @@
         <v>97.758462282398497</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -15934,7 +15999,7 @@
         <v>96.254186497443996</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -16002,7 +16067,7 @@
         <v>97.360248447204995</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -16070,7 +16135,7 @@
         <v>97.7628947368421</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -16138,7 +16203,7 @@
         <v>82.530303030303003</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -16206,7 +16271,7 @@
         <v>83.033480500367901</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -16274,7 +16339,7 @@
         <v>83.529411764705898</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -16342,7 +16407,7 @@
         <v>94.874779541446202</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -16410,7 +16475,7 @@
         <v>96.214937038645203</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -16478,7 +16543,7 @@
         <v>95.912921348314597</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -16546,7 +16611,7 @@
         <v>96.562992125984294</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -16614,7 +16679,7 @@
         <v>97.307632999229</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -16682,7 +16747,7 @@
         <v>96.921498661908998</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>34</v>
       </c>
@@ -16750,7 +16815,7 @@
         <v>97.314396887159504</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -16818,7 +16883,7 @@
         <v>97.249950288327696</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -16886,7 +16951,7 @@
         <v>97.640784982935202</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -16966,9 +17031,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16997,7 +17062,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -17026,7 +17091,7 @@
         <v>9.8204091615825398E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -17055,7 +17120,7 @@
         <v>1.8120125385497201</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -17084,7 +17149,7 @@
         <v>4.3387424108139996</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -17113,7 +17178,7 @@
         <v>15.1707390051837</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -17142,7 +17207,7 @@
         <v>7.7413503447952303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -17171,7 +17236,7 @@
         <v>0.74377576567497194</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -17200,7 +17265,7 @@
         <v>0.60327770651582502</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -17229,7 +17294,7 @@
         <v>0.87994077082994404</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -17258,7 +17323,7 @@
         <v>9.1271886011034091</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -17287,7 +17352,7 @@
         <v>2.07010055351626</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -17316,7 +17381,7 @@
         <v>0.33966973996470001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -17345,7 +17410,7 @@
         <v>0.58029997372854603</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -17374,7 +17439,7 @@
         <v>5.30333888632713</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -17403,7 +17468,7 @@
         <v>12.4425955746061</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -17432,7 +17497,7 @@
         <v>1.6061716999756901</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -17461,7 +17526,7 @@
         <v>0.26280183464137202</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -17490,7 +17555,7 @@
         <v>9.8059756095505701</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -17531,9 +17596,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -17580,7 +17645,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -17624,7 +17689,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -17668,7 +17733,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -17712,7 +17777,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -17756,7 +17821,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -17797,7 +17862,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -17838,7 +17903,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -17879,7 +17944,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -17920,7 +17985,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -17961,7 +18026,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -18002,7 +18067,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -18043,7 +18108,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -18084,7 +18149,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -18125,7 +18190,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -18166,7 +18231,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -18210,7 +18275,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -18254,7 +18319,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -18295,7 +18360,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>

</xml_diff>